<commit_message>
Update import_dmd2 to account for new structure of mapping spreadsheet
The numbers in the tests have changed because we've regenerated the
spreadsheet used in the test from the most recent mapping spreadsheet.
</commit_message>
<xml_diff>
--- a/openprescribing/dmd2/tests/data/bnf_code_mapping/mapping.xlsx
+++ b/openprescribing/dmd2/tests/data/bnf_code_mapping/mapping.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -361,7 +361,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>VMP / AMP</t>
+          <t>VMP / VMPP/ AMP / AMPP</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -386,7 +386,7 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>DM+D:Product and Pack Description</t>
+          <t>DM+D: Product and Pack Description</t>
         </is>
       </c>
     </row>
@@ -420,7 +420,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -447,7 +447,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -474,7 +474,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -533,7 +533,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -607,7 +607,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -730,7 +730,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -757,7 +757,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -779,7 +779,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -799,17 +799,12 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>'4744111000001109</t>
+          <t>'35894711000001106</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>Adenosine 6mg/2ml solution for injection vials</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Adenosine 6mg/2ml solution for injection 6 vials</t>
         </is>
       </c>
     </row>
@@ -821,7 +816,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -836,7 +831,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>'34516311000001106</t>
+          <t>'4744111000001109</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -846,46 +841,51 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection 5 vials</t>
+          <t>Adenosine 6mg/2ml solution for injection 6 vials</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>'0203020C0BBAAAA</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Adenocor_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>'4744411000001104</t>
+          <t>'34516311000001106</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection 5 vials</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -905,56 +905,56 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>'4744711000001105</t>
+          <t>'4744411000001104</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Adenocor 6mg/2ml solution for injection (Sanofi) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>'0203020C0AAAAAA</t>
+          <t>'0203020C0BBAAAA</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>Adenocor_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>'19663311000001109</t>
+          <t>'4744711000001105</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
+          <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Adenocor 6mg/2ml solution for injection (Sanofi) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -974,29 +974,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>'19663411000001102</t>
+          <t>'19663311000001109</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Adenosine 6mg/2ml solution for injection (Wockhardt UK Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1011,19 +1006,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>'20009311000001102</t>
+          <t>'19663411000001102</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (Wockhardt UK Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1043,29 +1043,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>'20009411000001109</t>
+          <t>'20009311000001102</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
           <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Adenosine 6mg/2ml solution for injection (A A H Pharmaceuticals Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1080,19 +1075,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>'21855411000001109</t>
+          <t>'20009411000001109</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Focus Pharmaceuticals Ltd)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (A A H Pharmaceuticals Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1112,29 +1112,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>'21855511000001108</t>
+          <t>'21855411000001109</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Focus Pharmaceuticals Ltd)</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Adenosine 6mg/2ml solution for injection (Focus Pharmaceuticals Ltd) 6 vials</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Advanz Pharma)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1149,19 +1144,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>'24530711000001102</t>
+          <t>'21855511000001108</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Advanz Pharma)</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (Advanz Pharma) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1181,29 +1181,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>'24531011000001108</t>
+          <t>'24530711000001102</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Adenosine 6mg/2ml solution for injection (Alliance Healthcare (Distribution) Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1218,19 +1213,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>'34516211000001103</t>
+          <t>'24531011000001108</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (Alliance Healthcare (Distribution) Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1250,17 +1250,12 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>'34516411000001104</t>
+          <t>'34516211000001103</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Adenosine 6mg/2ml solution for injection (Peckforton Pharmaceuticals Ltd) 5 vials</t>
         </is>
       </c>
     </row>
@@ -1272,39 +1267,39 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>'1106000X0AAAIAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Piloc HCl_Eye Dps 6%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>'9393611000001106</t>
+          <t>'34516411000001104</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops preservative free</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops preservative 1 ml</t>
+          <t>Adenosine 6mg/2ml solution for injection (Peckforton Pharmaceuticals Ltd) 5 vials</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1314,39 +1309,34 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>'1106000X0AAAIAI</t>
+          <t>'1106000X0AAA4A4</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Piloc HCl_Eye Dps 6%</t>
+          <t>Piloc HCl_Eye Dps 6% P/F</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>'20293311000001106</t>
+          <t>'36016311000001102</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>Pilocarpine hydrochloride 6% eye drops preservative free</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Pilocarpine hydrochloride 6% eye drops preservative 10 mls</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1361,12 +1351,17 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>'9393711000001102</t>
+          <t>'9393611000001106</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops preservative free (Special Order)</t>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative 1 ml</t>
         </is>
       </c>
     </row>
@@ -1378,7 +1373,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1393,24 +1388,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>'9393811000001105</t>
+          <t>'20293311000001106</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops preservative free (Special Order)</t>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops preservative (Special Order) 1 ml</t>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative 10 mls</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1430,49 +1425,49 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>'20293411000001104</t>
+          <t>'9393711000001102</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
           <t>Pilocarpine hydrochloride 6% eye drops preservative free (Special Order)</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Pilocarpine hydrochloride 6% eye drops preservative (Special Order) 10 mls</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>'1106000X0AAAIAI</t>
+          <t>'1106000X0AAA4A4</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Piloc HCl_Eye Dps 6%</t>
+          <t>Piloc HCl_Eye Dps 6% P/F</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>'347208002</t>
+          <t>'9393811000001105</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops</t>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free (Special Order)</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative (Special Order) 1 ml</t>
         </is>
       </c>
     </row>
@@ -1484,39 +1479,39 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>'1106000X0AAAIAI</t>
+          <t>'1106000X0AAA4A4</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Piloc HCl_Eye Dps 6%</t>
+          <t>Piloc HCl_Eye Dps 6% P/F</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>'9394111000001101</t>
+          <t>'20293411000001104</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops</t>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free (Special Order)</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye 1 ml</t>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative (Special Order) 10 mls</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1536,29 +1531,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>'20293111000001109</t>
+          <t>'347208002</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
           <t>Pilocarpine hydrochloride 6% eye drops</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Pilocarpine hydrochloride 6% eye 10 mls</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1573,12 +1563,17 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>'9394311000001104</t>
+          <t>'9394111000001101</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops (Special Order)</t>
+          <t>Pilocarpine hydrochloride 6% eye drops</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye 1 ml</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1585,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1605,24 +1600,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>'9394411000001106</t>
+          <t>'20293111000001109</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye drops (Special Order)</t>
+          <t>Pilocarpine hydrochloride 6% eye drops</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pilocarpine hydrochloride 6% eye (Special Order) 1 ml</t>
+          <t>Pilocarpine hydrochloride 6% eye 10 mls</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1642,49 +1637,49 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>'20293211000001103</t>
+          <t>'9394311000001104</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
           <t>Pilocarpine hydrochloride 6% eye drops (Special Order)</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Pilocarpine hydrochloride 6% eye (Special Order) 10 mls</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'1106000X0AAAIAI</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Piloc HCl_Eye Dps 6%</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>'22480211000001104</t>
+          <t>'9394411000001106</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
+          <t>Pilocarpine hydrochloride 6% eye drops (Special Order)</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye (Special Order) 1 ml</t>
         </is>
       </c>
     </row>
@@ -1696,39 +1691,39 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'1106000X0AAAIAI</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Piloc HCl_Eye Dps 6%</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>'22479411000001100</t>
+          <t>'20293211000001103</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
+          <t>Pilocarpine hydrochloride 6% eye drops (Special Order)</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% 50 grams</t>
+          <t>Pilocarpine hydrochloride 6% eye (Special Order) 10 mls</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1748,17 +1743,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>'22479511000001101</t>
+          <t>'22480211000001104</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
           <t>Diclofenac 2.32% gel</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Diclofenac 2.32% 30 grams</t>
         </is>
       </c>
     </row>
@@ -1770,7 +1760,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1785,7 +1775,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>'26352411000001101</t>
+          <t>'22479411000001100</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1795,39 +1785,44 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% 100 grams</t>
+          <t>Diclofenac 2.32% 50 grams</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'1003020U0AAAIAI</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Diclofenac Sod_Gel 2.32%</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>'22479611000001102</t>
+          <t>'22479511000001101</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% 30 grams</t>
         </is>
       </c>
     </row>
@@ -1839,39 +1834,39 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'1003020U0AAAIAI</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Diclofenac Sod_Gel 2.32%</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>'22479711000001106</t>
+          <t>'26352411000001101</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+          <t>Diclofenac 2.32% gel</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 50 grams</t>
+          <t>Diclofenac 2.32% 100 grams</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1891,17 +1886,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>'22479911000001108</t>
+          <t>'22479611000001102</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
           <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 30 grams</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1903,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1928,7 +1918,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>'26352611000001103</t>
+          <t>'22479711000001106</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1938,39 +1928,44 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 100 grams</t>
+          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 50 grams</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>'1305020C0AAFVFV</t>
+          <t>'1003020U0BBADAI</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>'28789311000001103</t>
+          <t>'22479911000001108</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream</t>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 30 grams</t>
         </is>
       </c>
     </row>
@@ -1982,32 +1977,32 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>'1305020C0AAFVFV</t>
+          <t>'1003020U0BBADAI</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>'28781611000001107</t>
+          <t>'26352611000001103</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream</t>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous 1 gram</t>
+          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 100 grams</t>
         </is>
       </c>
     </row>
@@ -2019,7 +2014,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMP</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2034,12 +2029,12 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>'28781711000001103</t>
+          <t>'28789311000001103</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream</t>
         </is>
       </c>
     </row>
@@ -2051,7 +2046,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMPP</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2066,17 +2061,17 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>'28781811000001106</t>
+          <t>'28781611000001107</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous (Special Order) 1 gram</t>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous 1 gram</t>
         </is>
       </c>
     </row>
@@ -2088,7 +2083,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2103,12 +2098,12 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>'28946311000001106</t>
+          <t>'28781711000001103</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream</t>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
         </is>
       </c>
     </row>
@@ -2120,7 +2115,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMPP</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2135,17 +2130,17 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>'28942411000001100</t>
+          <t>'28781811000001106</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream</t>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Coal tar 10% / Salicylic acid 5% in Aqueous 1 gram</t>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous (Special Order) 1 gram</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2152,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMP</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2172,12 +2167,12 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>'28942511000001101</t>
+          <t>'28946311000001106</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream</t>
         </is>
       </c>
     </row>
@@ -2189,30 +2184,99 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>VMPP</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>'28942411000001100</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous 1 gram</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>AMP</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>'1305020C0AAFVFV</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>'28942511000001101</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>AMPP</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
         <is>
           <t>'28942611000001102</t>
         </is>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="G57" t="inlineStr">
         <is>
           <t>Coal tar 10% / Salicylic acid 5% in Aqueous (Special Order) 1 gram</t>
         </is>

</xml_diff>